<commit_message>
DEV-10632 modified test_rosetta_fresh_load to match the column header changes within the data dictionary crosswalk
</commit_message>
<xml_diff>
--- a/usaspending_api/references/tests/data/20220517rosetta-test-file.xlsx
+++ b/usaspending_api/references/tests/data/20220517rosetta-test-file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sethstoudenmier/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayubshahab/Desktop/Ayub/usaspending/usaspending-api/usaspending_api/references/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3E4842-6ABB-3C44-A4D6-829C629C59F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468CCE27-3A6C-9544-9A40-4074664C114B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22940" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>DATA Act Information Model Schema (DAIMS)</t>
   </si>
@@ -165,22 +165,13 @@
     <t>Domain Values</t>
   </si>
   <si>
-    <t>Domain Values Code Description</t>
-  </si>
-  <si>
     <t>Award File</t>
   </si>
   <si>
     <t>Award Element</t>
   </si>
   <si>
-    <t>Subaward File</t>
-  </si>
-  <si>
     <t>Subaward Element</t>
-  </si>
-  <si>
-    <t>Account File</t>
   </si>
   <si>
     <t>Account Element</t>
@@ -310,6 +301,18 @@
       </rPr>
       <t xml:space="preserve"> to match USAspending values for the following data elements: ObligationsUndeliveredOrdersUnpaidTotal_CPE, ObligationsUndeliveredOrdersUnpaidTotal_FYB, USSGL480100_UndeliveredOrdersObligationsUnpaid_CPE, USSGL480100_UndeliveredOrdersObligationsUnpaid_FYB, USSGL488100_UpwardAdjustmentsOfPriorYearUndeliveredOrdersObligationsUnpaid_CPE, ObligationsDeliveredOrdersUnpaidTotal_CPE, ObligationsDeliveredOrdersUnpaidTotal_FYB, USSGL490100_DeliveredOrdersObligationsUnpaid_CPE, USSGL490100_DeliveredOrdersObligationsUnpaid_FYB, USSGL498100_UpwardAdjustmentsOfPriorYearDeliveredOrdersObligationsUnpaid_CPE, GrossOutlayAmountByProgramObjectClass_FYB, GrossOutlaysUndeliveredOrdersPrepaidTotal_CPE, GrossOutlaysUndeliveredOrdersPrepaidTotal_FYB, USSGL488200_UpwardAdjustmentsOfPriorYearUndeliveredOrdersObligationsPrepaidAdvanced_CPE, GrossOutlaysDeliveredOrdersPaidTotal_CPE, GrossOutlaysDeliveredOrdersPaidTotal_FYB, USSGL490200_DeliveredOrdersObligationsPaid_CPE, USSGL490800_AuthorityOutlayedNotYetDisbursed_CPE, USSGL490800_AuthorityOutlayedNotYetDisbursed_FYB, USSGL498200_UpwardAdjustmentsOfPriorYearDeliveredOrdersObligationsPaid_CPE, USSGL487100_DownwardAdjustmentsOfPriorYearUnpaidUndeliveredOrdersObligationsRecoveries_CPE, USSGL497100_DownwardAdjustmentsOfPriorYearUnpaidDeliveredOrdersObligationsRecoveries_CPE, USSGL487200_DownwardAdjustmentsOfPriorYearPrepaidAdvancedUndeliveredOrdersObligationsRefundsCollected_CPE, USSGL497200_DownwardAdjustmentsOfPriorYearPaidDeliveredOrdersObligationsRefundsCollected_CPE, USSGL483100_UndeliveredOrdersObligationsTransferredUnpaid_CPE, USSGL493100_DeliveredOrdersObligationsTransferredUnpaid_CPE, USSGL483200_UndeliveredOrdersObligationsTransferredPrepaidAdvanced_CPE, USSGL480200_UndeliveredOrdersObligationsPrepaidAdvanced_CPE, USSGL480200_UndeliveredOrdersObligationsPrepaidAdvanced_FYB</t>
     </r>
+  </si>
+  <si>
+    <t>Domain Values Code Desc</t>
+  </si>
+  <si>
+    <t>Award File (no time stamp)</t>
+  </si>
+  <si>
+    <t>Subaward File (no time stamp)</t>
+  </si>
+  <si>
+    <t>Account File (no time stamp)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,9 +656,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -866,7 +866,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Change Log Internal"/>
@@ -1610,22 +1610,22 @@
         <v>32</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="186" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="39" t="s">
-        <v>64</v>
+      <c r="D12" s="22" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="186.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="39" t="s">
-        <v>65</v>
+      <c r="D13" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1643,7 +1643,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1664,31 +1664,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="44" t="s">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="41"/>
+      <c r="O1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="42"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
@@ -1707,93 +1707,93 @@
         <v>42</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G2" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="I2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="K2" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="30" t="s">
-        <v>50</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>38</v>
       </c>
       <c r="O2" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="Q2" s="31" t="s">
         <v>45</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="F3" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="32" t="s">
+      <c r="G3" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="H3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="I3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="N3" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="O3" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="32" t="s">
+      <c r="P3" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>61</v>
-      </c>
       <c r="Q3" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1806,4 +1806,10 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{3de9faa6-9fe1-49b3-9a08-227a296b54a6}" enabled="1" method="Privileged" siteId="{d5fe813e-0caa-432a-b2ac-d555aa91bd1c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>